<commit_message>
working on process, changed in states
</commit_message>
<xml_diff>
--- a/Simu_Project/Documentation/table_helper.xlsx
+++ b/Simu_Project/Documentation/table_helper.xlsx
@@ -106,7 +106,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -123,11 +123,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -141,12 +147,16 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -165,13 +175,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C3:F12" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C3:F12" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
   <autoFilter ref="C3:F12"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Stream" dataDxfId="3"/>
-    <tableColumn id="2" name="Description" dataDxfId="2"/>
-    <tableColumn id="3" name="Distribution"/>
-    <tableColumn id="4" name="Mean Value" dataDxfId="1"/>
+    <tableColumn id="1" name="Stream" dataDxfId="5"/>
+    <tableColumn id="2" name="Description" dataDxfId="4"/>
+    <tableColumn id="3" name="Distribution" dataDxfId="3"/>
+    <tableColumn id="4" name="Mean Value" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -443,14 +453,14 @@
   <dimension ref="C3:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="32.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="6" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
@@ -472,13 +482,13 @@
       <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="3">
+      <c r="E4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1">
         <v>6</v>
       </c>
     </row>
@@ -486,13 +496,13 @@
       <c r="C5" s="1">
         <v>2</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="3">
+      <c r="E5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1">
         <v>4</v>
       </c>
     </row>
@@ -500,13 +510,13 @@
       <c r="C6" s="1">
         <v>3</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="3">
+      <c r="E6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1">
         <v>5</v>
       </c>
     </row>
@@ -514,13 +524,13 @@
       <c r="C7" s="1">
         <v>4</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="3">
+      <c r="E7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1">
         <v>5</v>
       </c>
     </row>
@@ -528,13 +538,13 @@
       <c r="C8" s="1">
         <v>5</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="3">
+      <c r="E8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="1">
         <v>8</v>
       </c>
       <c r="J8" s="2"/>
@@ -543,13 +553,13 @@
       <c r="C9" s="1">
         <v>6</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="3">
+      <c r="E9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="1">
         <v>12</v>
       </c>
     </row>
@@ -557,13 +567,13 @@
       <c r="C10" s="1">
         <v>7</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="3">
+      <c r="E10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1">
         <v>10</v>
       </c>
     </row>
@@ -571,13 +581,13 @@
       <c r="C11" s="1">
         <v>8</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="1">
         <v>0.05</v>
       </c>
     </row>
@@ -585,13 +595,13 @@
       <c r="C12" s="1">
         <v>9</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="1">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>